<commit_message>
Agregar Funcionalidad Mercadeo/OT - Resolver Bug
</commit_message>
<xml_diff>
--- a/Api/config/Plantilla_Implementaciones.xlsx
+++ b/Api/config/Plantilla_Implementaciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bullmarketingsas-my.sharepoint.com/personal/santiago_parraga_bullmarketing_com_co/Documents/Documentos/DesarrolloWeb/Terpel_Prbs_backup/Terpel_Prbs/Api/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="14_{93274129-114F-44F0-8C47-7853BBAF3F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AC3801D-CC1A-4A2B-8969-E69D6144A0A7}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="14_{93274129-114F-44F0-8C47-7853BBAF3F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{585B033E-F971-4474-A1F5-738445F74560}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{8029ABB4-7B01-4197-A985-FBC98B70FA5E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8029ABB4-7B01-4197-A985-FBC98B70FA5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte" sheetId="10" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Segmento</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Tipo Actividad</t>
+  </si>
+  <si>
+    <t>ID Registro</t>
   </si>
 </sst>
 </file>
@@ -350,6 +353,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -676,30 +683,30 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="9.5546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="25.109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="9.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="25.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="2" customWidth="1"/>
     <col min="13" max="13" width="46" style="2" customWidth="1"/>
-    <col min="14" max="14" width="25.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="24.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="25" style="2" customWidth="1"/>
-    <col min="21" max="21" width="24.33203125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="24.28515625" style="2" customWidth="1"/>
     <col min="22" max="22" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="11.44140625" style="1"/>
+    <col min="23" max="23" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -721,7 +728,7 @@
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" spans="2:24" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
         <v>11</v>
       </c>
@@ -747,7 +754,7 @@
       <c r="V2" s="8"/>
       <c r="W2" s="8"/>
     </row>
-    <row r="3" spans="2:24" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:24" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -769,7 +776,7 @@
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -825,7 +832,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="2:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="12"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
@@ -844,7 +851,7 @@
       <c r="Q5" s="14"/>
       <c r="R5" s="16"/>
     </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="X10" s="7"/>
     </row>
   </sheetData>
@@ -860,35 +867,37 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B1:AC10"/>
+  <dimension ref="B1:AD10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="9.5546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="25.109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5546875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="46" style="2" customWidth="1"/>
-    <col min="15" max="15" width="25.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="25.5546875" style="3" customWidth="1"/>
-    <col min="20" max="20" width="25.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="24.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="25" style="2" customWidth="1"/>
-    <col min="26" max="26" width="24.33203125" style="2" customWidth="1"/>
-    <col min="27" max="27" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="11.44140625" style="1"/>
+    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="9.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="25.140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5703125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="46" style="2" customWidth="1"/>
+    <col min="16" max="16" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="25.5703125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="25.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="25" style="2" customWidth="1"/>
+    <col min="27" max="27" width="24.28515625" style="2" customWidth="1"/>
+    <col min="28" max="28" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -914,8 +923,9 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="2:29" ht="18" x14ac:dyDescent="0.35">
+      <c r="AA1" s="1"/>
+    </row>
+    <row r="2" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
         <v>33</v>
       </c>
@@ -940,13 +950,14 @@
       <c r="U2" s="17"/>
       <c r="V2" s="17"/>
       <c r="W2" s="17"/>
-      <c r="X2" s="8"/>
+      <c r="X2" s="17"/>
       <c r="Y2" s="8"/>
       <c r="Z2" s="8"/>
       <c r="AA2" s="8"/>
       <c r="AB2" s="8"/>
-    </row>
-    <row r="3" spans="2:29" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC2" s="8"/>
+    </row>
+    <row r="3" spans="2:30" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -972,8 +983,9 @@
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
-    </row>
-    <row r="4" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="AA3" s="5"/>
+    </row>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -996,55 +1008,58 @@
         <v>18</v>
       </c>
       <c r="I4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="L4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="M4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="N4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="O4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="P4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="Q4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="10" t="s">
+      <c r="R4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="10" t="s">
+      <c r="S4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="S4" s="10" t="s">
+      <c r="T4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="10" t="s">
+      <c r="U4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="V4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="V4" s="10" t="s">
+      <c r="W4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="W4" s="11" t="s">
+      <c r="X4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
-    </row>
-    <row r="5" spans="2:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AA4" s="1"/>
+    </row>
+    <row r="5" spans="2:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="12"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
@@ -1055,9 +1070,9 @@
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
-      <c r="L5" s="15"/>
+      <c r="L5" s="14"/>
       <c r="M5" s="15"/>
-      <c r="N5" s="14"/>
+      <c r="N5" s="15"/>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
       <c r="Q5" s="14"/>
@@ -1066,14 +1081,15 @@
       <c r="T5" s="14"/>
       <c r="U5" s="14"/>
       <c r="V5" s="14"/>
-      <c r="W5" s="16"/>
-    </row>
-    <row r="10" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="AC10" s="7"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="16"/>
+    </row>
+    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AD10" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:W2"/>
+    <mergeCell ref="B2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se Ajusto en el rol de ot y mercadeo las dos implemtaciones 5, y se dejo solo el bonificador de segunda y tercera Implementacion
</commit_message>
<xml_diff>
--- a/Api/config/Plantilla_Implementaciones.xlsx
+++ b/Api/config/Plantilla_Implementaciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bullmarketingsas-my.sharepoint.com/personal/santiago_parraga_bullmarketing_com_co/Documents/Documentos/DesarrolloWeb/Terpel_Prbs_backup/Terpel_Prbs/Api/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bullmarketingsas-my.sharepoint.com/personal/santiago_parraga_bullmarketing_com_co/Documents/Documentos/DesarrolloWeb/Frotend_Git_Terpel/PlanChoqueNacional_/Api/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="14_{93274129-114F-44F0-8C47-7853BBAF3F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{585B033E-F971-4474-A1F5-738445F74560}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="14_{93274129-114F-44F0-8C47-7853BBAF3F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB483A48-7353-4E05-B7BB-354BADBD7F0C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8029ABB4-7B01-4197-A985-FBC98B70FA5E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8029ABB4-7B01-4197-A985-FBC98B70FA5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte" sheetId="10" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Segmento</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Implementacion por Punto de Venta</t>
   </si>
   <si>
-    <t>Quinta implementación</t>
-  </si>
-  <si>
     <t>NIT</t>
   </si>
   <si>
@@ -145,6 +142,12 @@
   </si>
   <si>
     <t>ID Registro</t>
+  </si>
+  <si>
+    <t>Quinta implementación 2</t>
+  </si>
+  <si>
+    <t>Quinta implementación 1</t>
   </si>
 </sst>
 </file>
@@ -353,10 +356,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -681,7 +680,7 @@
   </sheetPr>
   <dimension ref="B1:X10"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -748,7 +747,7 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="17"/>
       <c r="R2" s="17"/>
-      <c r="S2" s="8"/>
+      <c r="S2" s="17"/>
       <c r="T2" s="8"/>
       <c r="U2" s="8"/>
       <c r="V2" s="8"/>
@@ -784,7 +783,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>3</v>
@@ -796,19 +795,19 @@
         <v>0</v>
       </c>
       <c r="H4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>17</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M4" s="10" t="s">
         <v>6</v>
@@ -826,9 +825,11 @@
         <v>10</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
@@ -850,13 +851,14 @@
       <c r="P5" s="14"/>
       <c r="Q5" s="14"/>
       <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="X10" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:R2"/>
+    <mergeCell ref="B2:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -869,8 +871,8 @@
   </sheetPr>
   <dimension ref="B1:AD10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,7 +929,7 @@
     </row>
     <row r="2" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
@@ -993,7 +995,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>3</v>
@@ -1002,58 +1004,58 @@
         <v>1</v>
       </c>
       <c r="G4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="L4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="10" t="s">
+      <c r="N4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="O4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="Q4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" s="10" t="s">
+      <c r="R4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="10" t="s">
+      <c r="S4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="S4" s="10" t="s">
+      <c r="T4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="T4" s="10" t="s">
+      <c r="U4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="V4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="V4" s="10" t="s">
+      <c r="W4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="W4" s="10" t="s">
+      <c r="X4" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="X4" s="11" t="s">
-        <v>32</v>
       </c>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>

</xml_diff>

<commit_message>
Cambios Factor de Complejidad, Bonificacion, 5ta Implementacion (Fase_1, Fase_2)
</commit_message>
<xml_diff>
--- a/Api/config/Plantilla_Implementaciones.xlsx
+++ b/Api/config/Plantilla_Implementaciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bullmarketingsas-my.sharepoint.com/personal/santiago_parraga_bullmarketing_com_co/Documents/Documentos/DesarrolloWeb/Terpel_Prbs_backup/Terpel_Prbs/Api/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bullmarketingsas-my.sharepoint.com/personal/santiago_parraga_bullmarketing_com_co/Documents/Documentos/DesarrolloWeb/Frotend_Git_Terpel/PlanChoqueNacional_/Api/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="14_{93274129-114F-44F0-8C47-7853BBAF3F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{585B033E-F971-4474-A1F5-738445F74560}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="14_{93274129-114F-44F0-8C47-7853BBAF3F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB483A48-7353-4E05-B7BB-354BADBD7F0C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8029ABB4-7B01-4197-A985-FBC98B70FA5E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8029ABB4-7B01-4197-A985-FBC98B70FA5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte" sheetId="10" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Segmento</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Implementacion por Punto de Venta</t>
   </si>
   <si>
-    <t>Quinta implementación</t>
-  </si>
-  <si>
     <t>NIT</t>
   </si>
   <si>
@@ -145,6 +142,12 @@
   </si>
   <si>
     <t>ID Registro</t>
+  </si>
+  <si>
+    <t>Quinta implementación 2</t>
+  </si>
+  <si>
+    <t>Quinta implementación 1</t>
   </si>
 </sst>
 </file>
@@ -353,10 +356,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -681,7 +680,7 @@
   </sheetPr>
   <dimension ref="B1:X10"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -748,7 +747,7 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="17"/>
       <c r="R2" s="17"/>
-      <c r="S2" s="8"/>
+      <c r="S2" s="17"/>
       <c r="T2" s="8"/>
       <c r="U2" s="8"/>
       <c r="V2" s="8"/>
@@ -784,7 +783,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>3</v>
@@ -796,19 +795,19 @@
         <v>0</v>
       </c>
       <c r="H4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>17</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M4" s="10" t="s">
         <v>6</v>
@@ -826,9 +825,11 @@
         <v>10</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
@@ -850,13 +851,14 @@
       <c r="P5" s="14"/>
       <c r="Q5" s="14"/>
       <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="X10" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:R2"/>
+    <mergeCell ref="B2:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -869,8 +871,8 @@
   </sheetPr>
   <dimension ref="B1:AD10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,7 +929,7 @@
     </row>
     <row r="2" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
@@ -993,7 +995,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>3</v>
@@ -1002,58 +1004,58 @@
         <v>1</v>
       </c>
       <c r="G4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="L4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="10" t="s">
+      <c r="N4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="O4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="Q4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" s="10" t="s">
+      <c r="R4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="10" t="s">
+      <c r="S4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="S4" s="10" t="s">
+      <c r="T4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="T4" s="10" t="s">
+      <c r="U4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="V4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="V4" s="10" t="s">
+      <c r="W4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="W4" s="10" t="s">
+      <c r="X4" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="X4" s="11" t="s">
-        <v>32</v>
       </c>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>

</xml_diff>

<commit_message>
Agregar Columnas de Imp. 5_1,5_2
</commit_message>
<xml_diff>
--- a/Api/config/Plantilla_Implementaciones.xlsx
+++ b/Api/config/Plantilla_Implementaciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bullmarketingsas-my.sharepoint.com/personal/santiago_parraga_bullmarketing_com_co/Documents/Documentos/DesarrolloWeb/Terpel_Prbs_backup/Terpel_Prbs/Api/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bullmarketingsas-my.sharepoint.com/personal/santiago_parraga_bullmarketing_com_co/Documents/Documentos/DesarrolloWeb/Frotend_Git_Terpel/PlanChoqueNacional_/Api/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="14_{93274129-114F-44F0-8C47-7853BBAF3F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{585B033E-F971-4474-A1F5-738445F74560}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="14_{93274129-114F-44F0-8C47-7853BBAF3F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB483A48-7353-4E05-B7BB-354BADBD7F0C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8029ABB4-7B01-4197-A985-FBC98B70FA5E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8029ABB4-7B01-4197-A985-FBC98B70FA5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte" sheetId="10" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Segmento</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Implementacion por Punto de Venta</t>
   </si>
   <si>
-    <t>Quinta implementación</t>
-  </si>
-  <si>
     <t>NIT</t>
   </si>
   <si>
@@ -145,6 +142,12 @@
   </si>
   <si>
     <t>ID Registro</t>
+  </si>
+  <si>
+    <t>Quinta implementación 2</t>
+  </si>
+  <si>
+    <t>Quinta implementación 1</t>
   </si>
 </sst>
 </file>
@@ -353,10 +356,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -681,7 +680,7 @@
   </sheetPr>
   <dimension ref="B1:X10"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -748,7 +747,7 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="17"/>
       <c r="R2" s="17"/>
-      <c r="S2" s="8"/>
+      <c r="S2" s="17"/>
       <c r="T2" s="8"/>
       <c r="U2" s="8"/>
       <c r="V2" s="8"/>
@@ -784,7 +783,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>3</v>
@@ -796,19 +795,19 @@
         <v>0</v>
       </c>
       <c r="H4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>17</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M4" s="10" t="s">
         <v>6</v>
@@ -826,9 +825,11 @@
         <v>10</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
@@ -850,13 +851,14 @@
       <c r="P5" s="14"/>
       <c r="Q5" s="14"/>
       <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="X10" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:R2"/>
+    <mergeCell ref="B2:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -869,8 +871,8 @@
   </sheetPr>
   <dimension ref="B1:AD10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,7 +929,7 @@
     </row>
     <row r="2" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
@@ -993,7 +995,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>3</v>
@@ -1002,58 +1004,58 @@
         <v>1</v>
       </c>
       <c r="G4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="L4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="10" t="s">
+      <c r="N4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="O4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="Q4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" s="10" t="s">
+      <c r="R4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="10" t="s">
+      <c r="S4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="S4" s="10" t="s">
+      <c r="T4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="T4" s="10" t="s">
+      <c r="U4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="V4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="V4" s="10" t="s">
+      <c r="W4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="W4" s="10" t="s">
+      <c r="X4" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="X4" s="11" t="s">
-        <v>32</v>
       </c>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>

</xml_diff>